<commit_message>
Update with proliferation data
</commit_message>
<xml_diff>
--- a/NAD-NADH_proliferation_uncouple/annotation_df.xlsx
+++ b/NAD-NADH_proliferation_uncouple/annotation_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krdav/Google Drive/MCB/Sullivan_lab/lab-work/NAD-NADH_proliferation_uncouple/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F9ACC6-52AB-DD43-9C84-84853F175A2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E38827D-8A97-234C-97AD-4A62A3194829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6900" yWindow="1540" windowWidth="21660" windowHeight="16200" xr2:uid="{B348B963-32BD-DF42-ABAA-751E749D8A2A}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>1.3719002097481816</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -533,7 +533,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>1.3760887635139747</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -554,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>1.3642754662155234</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -575,7 +575,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>1.3683573211496605</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -595,7 +595,7 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>1.3673349283339424</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -615,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>1.3648672142025819</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -635,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>0.9</v>
+        <v>1.0685113476047834</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -655,7 +655,7 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>0.9</v>
+        <v>1.0835459285056379</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -675,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0.9</v>
+        <v>1.0552534968012119</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -695,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>0.1</v>
+        <v>0.14264426372740593</v>
       </c>
       <c r="G11" s="2"/>
     </row>
@@ -716,7 +716,7 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>0.1</v>
+        <v>0.16753990864725479</v>
       </c>
       <c r="G12" s="2"/>
     </row>
@@ -737,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>0.1</v>
+        <v>0.1618914352032011</v>
       </c>
       <c r="G13" s="2"/>
     </row>

</xml_diff>